<commit_message>
first steps in development
</commit_message>
<xml_diff>
--- a/data/iceland_basline_coordinates_caluclations.xlsx
+++ b/data/iceland_basline_coordinates_caluclations.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14760" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="12000" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -382,10 +382,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:L50"/>
+  <dimension ref="A2:L64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="L50" sqref="L50"/>
+    <sheetView tabSelected="1" topLeftCell="A45" workbookViewId="0">
+      <selection activeCell="L64" sqref="L64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -482,7 +482,7 @@
         <v>4.6399999999999997</v>
       </c>
       <c r="E4" s="1">
-        <f t="shared" ref="E4:E50" si="0">(B4+(((C4*60) + D4)/3600))</f>
+        <f t="shared" ref="E4:E64" si="0">(B4+(((C4*60) + D4)/3600))</f>
         <v>66.13462222222222</v>
       </c>
       <c r="G4" s="1">
@@ -495,11 +495,11 @@
         <v>48.81</v>
       </c>
       <c r="J4" s="1">
-        <f t="shared" ref="J4:J50" si="1">(-1)*(G4+(((H4*60) + I4)/3600))</f>
+        <f t="shared" ref="J4:J64" si="1">(-1)*(G4+(((H4*60) + I4)/3600))</f>
         <v>-20.180225</v>
       </c>
       <c r="L4" t="str">
-        <f t="shared" ref="L4:L50" si="2">CONCATENATE(J4, " , ", E4)</f>
+        <f t="shared" ref="L4:L64" si="2">CONCATENATE(J4, " , ", E4)</f>
         <v>-20,180225 , 66,1346222222222</v>
       </c>
     </row>
@@ -2111,6 +2111,501 @@
       <c r="L50" t="str">
         <f t="shared" si="2"/>
         <v>-22,4028305555556 , 66,4552027777778</v>
+      </c>
+    </row>
+    <row r="51" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="E51" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J51" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="L51" t="str">
+        <f t="shared" si="2"/>
+        <v>0 , 0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A52">
+        <v>1</v>
+      </c>
+      <c r="B52" s="1">
+        <v>66</v>
+      </c>
+      <c r="C52" s="1">
+        <v>34</v>
+      </c>
+      <c r="D52" s="1">
+        <v>3.27</v>
+      </c>
+      <c r="E52" s="1">
+        <f t="shared" si="0"/>
+        <v>66.567575000000005</v>
+      </c>
+      <c r="F52" s="1"/>
+      <c r="G52" s="1">
+        <v>18</v>
+      </c>
+      <c r="H52" s="1">
+        <v>1</v>
+      </c>
+      <c r="I52" s="1">
+        <v>18.739999999999998</v>
+      </c>
+      <c r="J52" s="1">
+        <f t="shared" si="1"/>
+        <v>-18.021872222222221</v>
+      </c>
+      <c r="K52" s="1"/>
+      <c r="L52" t="str">
+        <f t="shared" si="2"/>
+        <v>-18,0218722222222 , 66,567575</v>
+      </c>
+    </row>
+    <row r="53" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A53">
+        <v>2</v>
+      </c>
+      <c r="B53" s="1">
+        <v>66</v>
+      </c>
+      <c r="C53" s="1">
+        <v>33</v>
+      </c>
+      <c r="D53" s="1">
+        <v>33.72</v>
+      </c>
+      <c r="E53" s="1">
+        <f t="shared" si="0"/>
+        <v>66.559366666666662</v>
+      </c>
+      <c r="F53" s="1"/>
+      <c r="G53" s="1">
+        <v>18</v>
+      </c>
+      <c r="H53" s="1">
+        <v>0</v>
+      </c>
+      <c r="I53" s="1">
+        <v>3.65</v>
+      </c>
+      <c r="J53" s="1">
+        <f t="shared" si="1"/>
+        <v>-18.001013888888888</v>
+      </c>
+      <c r="K53" s="1"/>
+      <c r="L53" t="str">
+        <f t="shared" si="2"/>
+        <v>-18,0010138888889 , 66,5593666666667</v>
+      </c>
+    </row>
+    <row r="54" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A54">
+        <v>3</v>
+      </c>
+      <c r="B54" s="1">
+        <v>66</v>
+      </c>
+      <c r="C54" s="1">
+        <v>32</v>
+      </c>
+      <c r="D54" s="1">
+        <v>45.09</v>
+      </c>
+      <c r="E54" s="1">
+        <f t="shared" si="0"/>
+        <v>66.545858333333328</v>
+      </c>
+      <c r="F54" s="1"/>
+      <c r="G54" s="1">
+        <v>17</v>
+      </c>
+      <c r="H54" s="1">
+        <v>58</v>
+      </c>
+      <c r="I54" s="1">
+        <v>38.74</v>
+      </c>
+      <c r="J54" s="1">
+        <f t="shared" si="1"/>
+        <v>-17.977427777777777</v>
+      </c>
+      <c r="K54" s="1"/>
+      <c r="L54" t="str">
+        <f t="shared" si="2"/>
+        <v>-17,9774277777778 , 66,5458583333333</v>
+      </c>
+    </row>
+    <row r="55" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A55">
+        <v>4</v>
+      </c>
+      <c r="B55" s="1">
+        <v>66</v>
+      </c>
+      <c r="C55" s="1">
+        <v>32</v>
+      </c>
+      <c r="D55" s="1">
+        <v>0.88</v>
+      </c>
+      <c r="E55" s="1">
+        <f t="shared" si="0"/>
+        <v>66.533577777777779</v>
+      </c>
+      <c r="F55" s="1"/>
+      <c r="G55" s="1">
+        <v>17</v>
+      </c>
+      <c r="H55" s="1">
+        <v>58</v>
+      </c>
+      <c r="I55" s="1">
+        <v>40.369999999999997</v>
+      </c>
+      <c r="J55" s="1">
+        <f t="shared" si="1"/>
+        <v>-17.977880555555554</v>
+      </c>
+      <c r="K55" s="1"/>
+      <c r="L55" t="str">
+        <f t="shared" si="2"/>
+        <v>-17,9778805555556 , 66,5335777777778</v>
+      </c>
+    </row>
+    <row r="56" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A56">
+        <v>5</v>
+      </c>
+      <c r="B56" s="1">
+        <v>66</v>
+      </c>
+      <c r="C56" s="1">
+        <v>31</v>
+      </c>
+      <c r="D56" s="1">
+        <v>29.42</v>
+      </c>
+      <c r="E56" s="1">
+        <f t="shared" si="0"/>
+        <v>66.524838888888894</v>
+      </c>
+      <c r="F56" s="1"/>
+      <c r="G56" s="1">
+        <v>17</v>
+      </c>
+      <c r="H56" s="1">
+        <v>58</v>
+      </c>
+      <c r="I56" s="1">
+        <v>45.61</v>
+      </c>
+      <c r="J56" s="1">
+        <f t="shared" si="1"/>
+        <v>-17.97933611111111</v>
+      </c>
+      <c r="K56" s="1"/>
+      <c r="L56" t="str">
+        <f t="shared" si="2"/>
+        <v>-17,9793361111111 , 66,5248388888889</v>
+      </c>
+    </row>
+    <row r="57" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A57">
+        <v>6</v>
+      </c>
+      <c r="B57" s="1">
+        <v>66</v>
+      </c>
+      <c r="C57" s="1">
+        <v>31</v>
+      </c>
+      <c r="D57" s="1">
+        <v>36.26</v>
+      </c>
+      <c r="E57" s="1">
+        <f t="shared" si="0"/>
+        <v>66.526738888888886</v>
+      </c>
+      <c r="F57" s="1"/>
+      <c r="G57" s="1">
+        <v>17</v>
+      </c>
+      <c r="H57" s="1">
+        <v>59</v>
+      </c>
+      <c r="I57" s="1">
+        <v>24.84</v>
+      </c>
+      <c r="J57" s="1">
+        <f t="shared" si="1"/>
+        <v>-17.990233333333332</v>
+      </c>
+      <c r="K57" s="1"/>
+      <c r="L57" t="str">
+        <f t="shared" si="2"/>
+        <v>-17,9902333333333 , 66,5267388888889</v>
+      </c>
+    </row>
+    <row r="58" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A58">
+        <v>7</v>
+      </c>
+      <c r="B58" s="1">
+        <v>66</v>
+      </c>
+      <c r="C58" s="1">
+        <v>31</v>
+      </c>
+      <c r="D58" s="1">
+        <v>40.69</v>
+      </c>
+      <c r="E58" s="1">
+        <f t="shared" si="0"/>
+        <v>66.527969444444437</v>
+      </c>
+      <c r="F58" s="1"/>
+      <c r="G58" s="1">
+        <v>17</v>
+      </c>
+      <c r="H58" s="1">
+        <v>59</v>
+      </c>
+      <c r="I58" s="1">
+        <v>43.81</v>
+      </c>
+      <c r="J58" s="1">
+        <f t="shared" si="1"/>
+        <v>-17.995502777777777</v>
+      </c>
+      <c r="K58" s="1"/>
+      <c r="L58" t="str">
+        <f t="shared" si="2"/>
+        <v>-17,9955027777778 , 66,5279694444444</v>
+      </c>
+    </row>
+    <row r="59" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A59">
+        <v>8</v>
+      </c>
+      <c r="B59" s="1">
+        <v>66</v>
+      </c>
+      <c r="C59" s="1">
+        <v>32</v>
+      </c>
+      <c r="D59" s="1">
+        <v>15.6</v>
+      </c>
+      <c r="E59" s="1">
+        <f t="shared" si="0"/>
+        <v>66.537666666666667</v>
+      </c>
+      <c r="F59" s="1"/>
+      <c r="G59" s="1">
+        <v>18</v>
+      </c>
+      <c r="H59" s="1">
+        <v>1</v>
+      </c>
+      <c r="I59" s="1">
+        <v>17.25</v>
+      </c>
+      <c r="J59" s="1">
+        <f t="shared" si="1"/>
+        <v>-18.021458333333332</v>
+      </c>
+      <c r="K59" s="1"/>
+      <c r="L59" t="str">
+        <f t="shared" si="2"/>
+        <v>-18,0214583333333 , 66,5376666666667</v>
+      </c>
+    </row>
+    <row r="60" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A60">
+        <v>9</v>
+      </c>
+      <c r="B60" s="1">
+        <v>66</v>
+      </c>
+      <c r="C60" s="1">
+        <v>32</v>
+      </c>
+      <c r="D60" s="1">
+        <v>21.61</v>
+      </c>
+      <c r="E60" s="1">
+        <f t="shared" si="0"/>
+        <v>66.539336111111112</v>
+      </c>
+      <c r="F60" s="1"/>
+      <c r="G60" s="1">
+        <v>18</v>
+      </c>
+      <c r="H60" s="1">
+        <v>1</v>
+      </c>
+      <c r="I60" s="1">
+        <v>22.93</v>
+      </c>
+      <c r="J60" s="1">
+        <f t="shared" si="1"/>
+        <v>-18.023036111111111</v>
+      </c>
+      <c r="K60" s="1"/>
+      <c r="L60" t="str">
+        <f t="shared" si="2"/>
+        <v>-18,0230361111111 , 66,5393361111111</v>
+      </c>
+    </row>
+    <row r="61" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A61">
+        <v>10</v>
+      </c>
+      <c r="B61" s="1">
+        <v>66</v>
+      </c>
+      <c r="C61" s="1">
+        <v>32</v>
+      </c>
+      <c r="D61" s="1">
+        <v>33.57</v>
+      </c>
+      <c r="E61" s="1">
+        <f t="shared" si="0"/>
+        <v>66.542658333333335</v>
+      </c>
+      <c r="F61" s="1"/>
+      <c r="G61" s="1">
+        <v>18</v>
+      </c>
+      <c r="H61" s="1">
+        <v>1</v>
+      </c>
+      <c r="I61" s="1">
+        <v>34.450000000000003</v>
+      </c>
+      <c r="J61" s="1">
+        <f t="shared" si="1"/>
+        <v>-18.02623611111111</v>
+      </c>
+      <c r="K61" s="1"/>
+      <c r="L61" t="str">
+        <f t="shared" si="2"/>
+        <v>-18,0262361111111 , 66,5426583333333</v>
+      </c>
+    </row>
+    <row r="62" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A62">
+        <v>11</v>
+      </c>
+      <c r="B62" s="1">
+        <v>66</v>
+      </c>
+      <c r="C62" s="1">
+        <v>33</v>
+      </c>
+      <c r="D62" s="1">
+        <v>4.7699999999999996</v>
+      </c>
+      <c r="E62" s="1">
+        <f t="shared" si="0"/>
+        <v>66.551325000000006</v>
+      </c>
+      <c r="F62" s="1"/>
+      <c r="G62" s="1">
+        <v>18</v>
+      </c>
+      <c r="H62" s="1">
+        <v>1</v>
+      </c>
+      <c r="I62" s="1">
+        <v>48.6</v>
+      </c>
+      <c r="J62" s="1">
+        <f t="shared" si="1"/>
+        <v>-18.030166666666666</v>
+      </c>
+      <c r="K62" s="1"/>
+      <c r="L62" t="str">
+        <f t="shared" si="2"/>
+        <v>-18,0301666666667 , 66,551325</v>
+      </c>
+    </row>
+    <row r="63" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A63">
+        <v>12</v>
+      </c>
+      <c r="B63" s="1">
+        <v>66</v>
+      </c>
+      <c r="C63" s="1">
+        <v>34</v>
+      </c>
+      <c r="D63" s="1">
+        <v>1.34</v>
+      </c>
+      <c r="E63" s="1">
+        <f t="shared" si="0"/>
+        <v>66.567038888888888</v>
+      </c>
+      <c r="F63" s="1"/>
+      <c r="G63" s="1">
+        <v>18</v>
+      </c>
+      <c r="H63" s="1">
+        <v>1</v>
+      </c>
+      <c r="I63" s="1">
+        <v>28.13</v>
+      </c>
+      <c r="J63" s="1">
+        <f t="shared" si="1"/>
+        <v>-18.024480555555556</v>
+      </c>
+      <c r="K63" s="1"/>
+      <c r="L63" t="str">
+        <f t="shared" si="2"/>
+        <v>-18,0244805555556 , 66,5670388888889</v>
+      </c>
+    </row>
+    <row r="64" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A64">
+        <v>13</v>
+      </c>
+      <c r="B64" s="1">
+        <v>66</v>
+      </c>
+      <c r="C64" s="1">
+        <v>34</v>
+      </c>
+      <c r="D64" s="1">
+        <v>3.27</v>
+      </c>
+      <c r="E64" s="1">
+        <f t="shared" si="0"/>
+        <v>66.567575000000005</v>
+      </c>
+      <c r="F64" s="1"/>
+      <c r="G64" s="1">
+        <v>18</v>
+      </c>
+      <c r="H64" s="1">
+        <v>1</v>
+      </c>
+      <c r="I64" s="1">
+        <v>18.739999999999998</v>
+      </c>
+      <c r="J64" s="1">
+        <f t="shared" si="1"/>
+        <v>-18.021872222222221</v>
+      </c>
+      <c r="K64" s="1"/>
+      <c r="L64" t="str">
+        <f t="shared" si="2"/>
+        <v>-18,0218722222222 , 66,567575</v>
       </c>
     </row>
   </sheetData>

</xml_diff>